<commit_message>
Refactoring - unclassified lineages
</commit_message>
<xml_diff>
--- a/tabular/eve/parvovirinae/epv-dependo-side-data.xlsx
+++ b/tabular/eve/parvovirinae/epv-dependo-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/parvovirinae/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/parvovirinae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF1B43D-0739-8D4F-85BD-F47C56BA2E13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25321E2E-232F-7447-8F13-85B91FE7F041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16200" yWindow="500" windowWidth="35000" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="27980" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DONE" sheetId="2" r:id="rId1"/>
@@ -7379,8 +7379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG326"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>